<commit_message>
se agrego el diagrama de pert
</commit_message>
<xml_diff>
--- a/Historias de usuario_backlog_sprint_y_pert.xlsx
+++ b/Historias de usuario_backlog_sprint_y_pert.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja3" sheetId="3" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="134">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Tiempo pesimo(b)</t>
   </si>
   <si>
-    <t>Actividad presedente</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -129,12 +126,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>HISTORIA DE USUARIO</t>
   </si>
   <si>
@@ -652,9 +643,6 @@
     <t>Numero de Historia: 3</t>
   </si>
   <si>
-    <t>Numero de tarea:1.3</t>
-  </si>
-  <si>
     <r>
       <t>Nombre de la tarea:</t>
     </r>
@@ -1010,18 +998,12 @@
     </r>
   </si>
   <si>
-    <t>Numero de tarea:1.4</t>
-  </si>
-  <si>
     <t>Numero de tarea:1.5</t>
   </si>
   <si>
     <t>Numero de tarea:1.6</t>
   </si>
   <si>
-    <t>Numero de Historia: 6</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Nombre de la tarea: </t>
     </r>
@@ -1355,28 +1337,79 @@
     <t>registro de datos del inmuebles</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
+    <t>tiempo en dias</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>E,D</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>Tiempo estimado(te)</t>
+  </si>
+  <si>
+    <t>Tiempo estimado(te)=</t>
+  </si>
+  <si>
+    <t>(a+4m+b)/6</t>
+  </si>
+  <si>
+    <t>Varianza (o^2)</t>
+  </si>
+  <si>
+    <t>((b-a)/6)^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varinza </t>
+  </si>
+  <si>
+    <t xml:space="preserve">actividades criticas </t>
+  </si>
+  <si>
+    <t>36 dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duracion de proyecto </t>
+  </si>
+  <si>
+    <t>Desviacion estandar</t>
+  </si>
+  <si>
+    <t>probabilidad</t>
+  </si>
+  <si>
+    <t>calculo de la varianza</t>
+  </si>
+  <si>
+    <t>o^2=</t>
+  </si>
+  <si>
+    <t>o=</t>
+  </si>
+  <si>
+    <t>Numero de tarea:2.1</t>
+  </si>
+  <si>
+    <t>Tiempo mas probable (m)</t>
+  </si>
+  <si>
+    <t>Actividad precedente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1408,12 +1441,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1432,19 +1459,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1472,19 +1501,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1597,43 +1638,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1698,11 +1702,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF16365C"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF16365C"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF16365C"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1731,25 +1776,19 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1758,113 +1797,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2172,813 +2243,758 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86:D87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="55.109375" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="44.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="32" t="s">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="E3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="2:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="E5" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="E3" s="28" t="s">
+      <c r="C6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="E7" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="2:7" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="E8" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="E12" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="28"/>
+    </row>
+    <row r="13" spans="2:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="E14" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="E16" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="2:6" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="E17" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="40"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="30"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="20"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="20"/>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="20"/>
+    </row>
+    <row r="22" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="E22" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="E24" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="30"/>
+    </row>
+    <row r="25" spans="2:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="E26" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="2:6" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="E27" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="40"/>
+    </row>
+    <row r="28" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="30"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="20"/>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="20"/>
+    </row>
+    <row r="31" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="42"/>
+      <c r="E31" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="28"/>
+    </row>
+    <row r="32" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="E33" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="30"/>
+    </row>
+    <row r="34" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="E35" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="30"/>
+    </row>
+    <row r="36" spans="2:6" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="E36" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="40"/>
+    </row>
+    <row r="37" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="30"/>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="20"/>
+    </row>
+    <row r="39" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="42"/>
+      <c r="E39" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="30"/>
+      <c r="E41" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="30"/>
+    </row>
+    <row r="42" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" spans="2:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="C42" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="E42" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="E5" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="31"/>
-    </row>
-    <row r="6" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="C43" s="30"/>
+      <c r="E43" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" s="30"/>
+    </row>
+    <row r="44" spans="2:6" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="30"/>
+      <c r="E44" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="40"/>
+    </row>
+    <row r="45" spans="2:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="E7" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="31"/>
-    </row>
-    <row r="8" spans="2:7" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="30" t="s">
+      <c r="C45" s="30"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="20"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="20"/>
+    </row>
+    <row r="48" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="42"/>
+      <c r="E48" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="28"/>
+    </row>
+    <row r="49" spans="2:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="30"/>
+      <c r="E50" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F50" s="30"/>
+    </row>
+    <row r="51" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="E52" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="30"/>
+    </row>
+    <row r="53" spans="2:6" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="30"/>
+      <c r="E53" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F53" s="40"/>
+    </row>
+    <row r="54" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="30"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="20"/>
+    </row>
+    <row r="56" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="36"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="36"/>
+    </row>
+    <row r="57" spans="2:6" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" s="23"/>
+      <c r="E57" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="38"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="F58" s="38"/>
+    </row>
+    <row r="59" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="23"/>
+      <c r="E59" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F59" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="38"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="38"/>
+    </row>
+    <row r="61" spans="2:6" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="38"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F61" s="34"/>
+    </row>
+    <row r="62" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="38"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="20"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="20"/>
+    </row>
+    <row r="65" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="20"/>
+    </row>
+    <row r="66" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="36"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F66" s="36"/>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" s="23"/>
+      <c r="E67" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F67" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" s="38"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="F68" s="38"/>
+    </row>
+    <row r="69" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="E8" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="24"/>
-    </row>
-    <row r="9" spans="2:7" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="E9" t="s">
+      <c r="C69" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="23"/>
+      <c r="E69" s="24" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="E12" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="2:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="F69" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="31"/>
-      <c r="E14" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="31"/>
-    </row>
-    <row r="15" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="C70" s="38"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="F70" s="38"/>
+    </row>
+    <row r="71" spans="2:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" s="38"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F71" s="34"/>
+    </row>
+    <row r="72" spans="2:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="31"/>
-      <c r="E16" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="31"/>
-    </row>
-    <row r="17" spans="2:6" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="31"/>
-      <c r="E17" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="27"/>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="31"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="23"/>
-    </row>
-    <row r="22" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="33"/>
-      <c r="E22" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="29"/>
-    </row>
-    <row r="23" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="22" t="s">
+      <c r="C72" s="38"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+    </row>
+    <row r="73" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C75" s="42"/>
+      <c r="E75" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="28"/>
+    </row>
+    <row r="76" spans="2:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="30"/>
+      <c r="E77" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F77" s="30"/>
+    </row>
+    <row r="78" spans="2:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F78" s="19" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="31"/>
-      <c r="E24" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="31"/>
-    </row>
-    <row r="25" spans="2:6" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="22" t="s">
+    <row r="79" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C79" s="30"/>
+      <c r="E79" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F79" s="30"/>
+    </row>
+    <row r="80" spans="2:6" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C80" s="30"/>
+      <c r="E80" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F80" s="32"/>
+    </row>
+    <row r="81" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="31"/>
-      <c r="E26" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="31"/>
-    </row>
-    <row r="27" spans="2:6" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="E27" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="27"/>
-    </row>
-    <row r="28" spans="2:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="31"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="23"/>
-    </row>
-    <row r="30" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="23"/>
-    </row>
-    <row r="31" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="33"/>
-      <c r="E31" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="29"/>
-    </row>
-    <row r="32" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="E33" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" s="31"/>
-    </row>
-    <row r="34" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="31"/>
-      <c r="E35" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="31"/>
-    </row>
-    <row r="36" spans="2:6" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="E36" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="27"/>
-    </row>
-    <row r="37" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="31"/>
-    </row>
-    <row r="38" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="23"/>
-    </row>
-    <row r="39" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="33"/>
-      <c r="E39" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F39" s="29"/>
-    </row>
-    <row r="40" spans="2:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="31"/>
-      <c r="E41" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="F41" s="31"/>
-    </row>
-    <row r="42" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="31"/>
-      <c r="E43" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="31"/>
-    </row>
-    <row r="44" spans="2:6" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="31"/>
-      <c r="E44" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="F44" s="27"/>
-    </row>
-    <row r="45" spans="2:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="31"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="23"/>
-    </row>
-    <row r="47" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="23"/>
-    </row>
-    <row r="48" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="33"/>
-      <c r="E48" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F48" s="29"/>
-    </row>
-    <row r="49" spans="2:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="31"/>
-      <c r="E50" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" s="31"/>
-    </row>
-    <row r="51" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F51" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="31"/>
-      <c r="E52" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F52" s="31"/>
-    </row>
-    <row r="53" spans="2:6" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="31"/>
-      <c r="E53" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="F53" s="27"/>
-    </row>
-    <row r="54" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C54" s="31"/>
-    </row>
-    <row r="55" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="23"/>
-    </row>
-    <row r="56" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="38"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="F56" s="38"/>
-    </row>
-    <row r="57" spans="2:6" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D57" s="39"/>
-      <c r="E57" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="F57" s="41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="F58" s="43"/>
-    </row>
-    <row r="59" spans="2:6" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D59" s="39"/>
-      <c r="E59" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F59" s="41" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="43"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="F60" s="43"/>
-    </row>
-    <row r="61" spans="2:6" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C61" s="43"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="F61" s="45"/>
-    </row>
-    <row r="62" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C62" s="43"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B63" s="23"/>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="23"/>
-    </row>
-    <row r="65" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="23"/>
-    </row>
-    <row r="66" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C66" s="38"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="F66" s="38"/>
-    </row>
-    <row r="67" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D67" s="39"/>
-      <c r="E67" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="F67" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" s="43"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="F68" s="43"/>
-    </row>
-    <row r="69" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C69" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D69" s="39"/>
-      <c r="E69" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F69" s="41" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C70" s="43"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="F70" s="43"/>
-    </row>
-    <row r="71" spans="2:6" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C71" s="43"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="F71" s="45"/>
-    </row>
-    <row r="72" spans="2:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C72" s="43"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="39"/>
-    </row>
-    <row r="73" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="2:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C75" s="33"/>
-      <c r="E75" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F75" s="29"/>
-    </row>
-    <row r="76" spans="2:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E76" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F76" s="22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C77" s="31"/>
-      <c r="E77" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="F77" s="31"/>
-    </row>
-    <row r="78" spans="2:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E78" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F78" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C79" s="31"/>
-      <c r="E79" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F79" s="31"/>
-    </row>
-    <row r="80" spans="2:6" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C80" s="31"/>
-      <c r="E80" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="F80" s="47"/>
-    </row>
-    <row r="81" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C81" s="31"/>
+      <c r="C81" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B81:C81"/>
@@ -2995,11 +3011,66 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B77:C77"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3011,58 +3082,61 @@
   <dimension ref="B2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L5" sqref="L5:L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="34" t="s">
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-    </row>
-    <row r="4" spans="2:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
+    </row>
+    <row r="4" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="52" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J4" s="51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -3075,7 +3149,9 @@
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="43">
+        <v>1</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="9">
         <v>43235</v>
@@ -3084,16 +3160,17 @@
         <f>H5+5</f>
         <v>43240</v>
       </c>
-      <c r="J5" s="56" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="26">
+        <f>I5-H5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
@@ -3101,23 +3178,22 @@
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="11">
-        <v>1</v>
-      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="17">
+      <c r="H6" s="15">
         <f>I5</f>
         <v>43240</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="15">
         <f>H6+5</f>
         <v>43245</v>
       </c>
-      <c r="J6" s="56" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J6" s="26">
+        <f>I6-H6</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>3</v>
       </c>
@@ -3130,23 +3206,24 @@
       <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="43">
         <v>2</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="17">
+      <c r="H7" s="15">
         <f>I6+1</f>
         <v>43246</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="15">
         <f>H7+3</f>
         <v>43249</v>
       </c>
-      <c r="J7" s="56" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J7" s="26">
+        <f>I7-H7</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -3159,140 +3236,124 @@
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="49"/>
+      <c r="F8" s="44"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="17">
+      <c r="H8" s="15">
+        <f>I7</f>
         <v>43249</v>
       </c>
       <c r="I8" s="9">
         <f>H8+3</f>
         <v>43252</v>
       </c>
-      <c r="J8" s="56" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="48"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="56"/>
-    </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="48"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="56"/>
-    </row>
-    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J8" s="26">
+        <f>I8-H8</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="45">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="15">
+        <f>I8+1</f>
+        <v>43253</v>
+      </c>
+      <c r="I9" s="15">
+        <f>H9+10</f>
+        <v>43263</v>
+      </c>
+      <c r="J9" s="26">
+        <f>I9-H9</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="46">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="15">
+        <f>I9+1</f>
+        <v>43264</v>
+      </c>
+      <c r="I10" s="9">
+        <f>H10+6</f>
+        <v>43270</v>
+      </c>
+      <c r="J10" s="26">
+        <f>I10-H10</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="51">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="47"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="17">
-        <v>43264</v>
-      </c>
-      <c r="I11" s="17">
-        <f>H11+13</f>
+      <c r="H11" s="9">
+        <f>I10</f>
+        <v>43270</v>
+      </c>
+      <c r="I11" s="9">
+        <f>H11+7</f>
         <v>43277</v>
       </c>
-      <c r="J11" s="56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="1">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="17">
-        <f>I11+1</f>
-        <v>43278</v>
-      </c>
-      <c r="I12" s="9">
-        <f>H12+5</f>
-        <v>43283</v>
-      </c>
-      <c r="J12" s="56" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="48"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="54">
-        <v>4</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="56"/>
-    </row>
-    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="1">
+      <c r="J11" s="26">
+        <f>I11-H11</f>
         <v>7</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="9">
-        <f>I12</f>
-        <v>43283</v>
-      </c>
-      <c r="I14" s="9">
-        <f>H14+4</f>
-        <v>43287</v>
-      </c>
-      <c r="J14" s="56" t="s">
-        <v>122</v>
-      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3301,157 +3362,495 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F18"/>
+  <dimension ref="A2:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
+    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" s="54" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C12" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D12" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="55">
+        <v>4</v>
+      </c>
+      <c r="D13" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="55">
+        <v>5</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="55">
+        <v>4</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="55">
+        <v>5</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="55">
+        <v>2</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="55">
+        <v>4</v>
+      </c>
+      <c r="F15" s="55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="55">
+        <v>2</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="55">
+        <v>3</v>
+      </c>
+      <c r="F16" s="55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="55">
+        <v>8</v>
+      </c>
+      <c r="D17" s="55">
+        <v>9</v>
+      </c>
+      <c r="E17" s="55">
+        <v>10</v>
+      </c>
+      <c r="F17" s="55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="55">
+        <v>4</v>
+      </c>
+      <c r="D18" s="55">
+        <v>5</v>
+      </c>
+      <c r="E18" s="55">
+        <v>6</v>
+      </c>
+      <c r="F18" s="55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="55">
+        <v>6</v>
+      </c>
+      <c r="E19" s="55">
+        <v>7</v>
+      </c>
+      <c r="F19" s="55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>A13+A14+A15+A16+A17+A18+A19</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E22" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F22" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="C23" s="55">
+        <v>5</v>
+      </c>
+      <c r="D23" s="55">
+        <v>6</v>
+      </c>
+      <c r="E23" s="55">
+        <v>8</v>
+      </c>
+      <c r="F23" s="58">
+        <f>(C23+4*D23+E23)/6</f>
+        <v>6.166666666666667</v>
+      </c>
+      <c r="G23" s="58">
+        <f>((C23-E23)/6)^2</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="25" t="s">
+      <c r="C24" s="55">
+        <v>5</v>
+      </c>
+      <c r="D24" s="55">
+        <v>6.5</v>
+      </c>
+      <c r="E24" s="55">
+        <v>7</v>
+      </c>
+      <c r="F24" s="58">
+        <f>(C24+4*D24+E24)/6</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="G24" s="58">
+        <f>((C24-E24)/6)^2</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="25" t="s">
+      <c r="C25" s="55">
+        <v>3</v>
+      </c>
+      <c r="D25" s="55">
+        <v>4</v>
+      </c>
+      <c r="E25" s="55">
+        <v>5</v>
+      </c>
+      <c r="F25" s="58">
+        <f>(C25+4*D25+E25)/6</f>
+        <v>4</v>
+      </c>
+      <c r="G25" s="58">
+        <f t="shared" ref="G24:G29" si="0">((C25-E25)/6)^2</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
+      <c r="C26" s="55">
+        <v>2.7</v>
+      </c>
+      <c r="D26" s="55">
+        <v>3</v>
+      </c>
+      <c r="E26" s="55">
+        <v>4</v>
+      </c>
+      <c r="F26" s="58">
+        <f t="shared" ref="F25:F29" si="1">(C26+4*D26+E26)/6</f>
+        <v>3.1166666666666667</v>
+      </c>
+      <c r="G26" s="58">
+        <f t="shared" si="0"/>
+        <v>4.6944444444444434E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="25" t="s">
+      <c r="C27" s="55">
+        <v>10</v>
+      </c>
+      <c r="D27" s="55">
+        <v>11</v>
+      </c>
+      <c r="E27" s="55">
+        <v>13</v>
+      </c>
+      <c r="F27" s="58">
+        <f t="shared" si="1"/>
+        <v>11.166666666666666</v>
+      </c>
+      <c r="G27" s="58">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
+      <c r="C28" s="55">
+        <v>6</v>
+      </c>
+      <c r="D28" s="55">
+        <v>7</v>
+      </c>
+      <c r="E28" s="55">
+        <v>9</v>
+      </c>
+      <c r="F28" s="58">
+        <f t="shared" si="1"/>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="G28" s="58">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="C29" s="55">
+        <v>7</v>
+      </c>
+      <c r="D29" s="55">
+        <v>8</v>
+      </c>
+      <c r="E29" s="55">
+        <v>9</v>
+      </c>
+      <c r="F29" s="58">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G29" s="58">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="63"/>
+      <c r="B32" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="58">
+        <f>(C23+4*D23+E23)/6</f>
+        <v>6.166666666666667</v>
+      </c>
+      <c r="D33" s="58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="58">
+        <f>(C25+4*D25+E25)/6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="58">
+        <f>(C27+4*D27+E27)/6</f>
+        <v>11.166666666666666</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="58">
+        <f>(C28+4*D28+E28)/6</f>
+        <v>7.166666666666667</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="58">
+        <f>(C29+4*D29+E29)/6</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="59"/>
+      <c r="E39" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="G39" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="H39" s="61"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41">
+        <f>G23+G25+G27+G28+G29</f>
+        <v>0.97222222222222232</v>
+      </c>
+      <c r="D41" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41">
+        <f>SQRT(C41)</f>
+        <v>0.98601329718326935</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="G39:H39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>